<commit_message>
RV13: Elastic Net con Estrato + receta RV10
</commit_message>
<xml_diff>
--- a/Contabilidad modelos.xlsx
+++ b/Contabilidad modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\TODO\UNI ANDES\SEM 8 (2024-1)\Big Data y Machine Learning\Taller 3\BDML_2024_PS_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC094D-F6BC-45D3-988E-D0667EA9EC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAD505E-BACB-46F9-A9C4-162B42B85D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4CAA7325-4791-4168-8C9B-C73AA3489A20}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>No.</t>
   </si>
@@ -257,7 +257,18 @@
               terraza, ascensor, estrato,</t>
   </si>
   <si>
-    <t>Penalty: 0,01; mixture: 2</t>
+    <t>Penalty: 0,01; mixture: 0</t>
+  </si>
+  <si>
+    <t>property_type,  area, dist_nearest_restaurant,
+              dist_nearest_parques, baños, n_pisos_numerico,dist_nearest_universidades,
+              terraza, remodelado, estrato</t>
+  </si>
+  <si>
+    <t>rec1 &lt;- recipe(base_train) %&gt;%
+  update_role(property_type,  area, dist_nearest_restaurant,
+              dist_nearest_parques, baños, n_pisos_numerico,dist_nearest_universidades,
+              terraza, remodelado, estrato,</t>
   </si>
 </sst>
 </file>
@@ -319,11 +330,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -659,11 +671,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B44E75D-B032-48F0-BA17-754A2F99A73B}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,7 +685,7 @@
     <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -695,10 +707,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -776,7 +788,6 @@
       <c r="G4" s="2">
         <v>159926333</v>
       </c>
-      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -800,7 +811,6 @@
       <c r="G5" s="2">
         <v>165197347</v>
       </c>
-      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -824,7 +834,6 @@
       <c r="G6" s="2">
         <v>155316466</v>
       </c>
-      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -845,7 +854,6 @@
       <c r="G7" s="2">
         <v>156457892</v>
       </c>
-      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -921,13 +929,12 @@
       <c r="G10" s="2">
         <v>153274279</v>
       </c>
-      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C11" t="s">
@@ -979,10 +986,10 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
       <c r="D13" t="s">
@@ -1001,8 +1008,82 @@
         <v>202034162</v>
       </c>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2">
+        <v>152163580</v>
+      </c>
+      <c r="H14" s="2">
+        <v>202821306</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="G2:G13">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
RV15: XGBoost v2 (excel completo)
</commit_message>
<xml_diff>
--- a/Contabilidad modelos.xlsx
+++ b/Contabilidad modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\TODO\UNI ANDES\SEM 8 (2024-1)\Big Data y Machine Learning\Taller 3\BDML_2024_PS_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7189BCDC-E622-4442-B847-9BC55D2DE617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C47865-1E1C-483A-B234-BA27BC34EA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4CAA7325-4791-4168-8C9B-C73AA3489A20}"/>
   </bookViews>
@@ -702,8 +702,8 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1110,6 +1110,9 @@
       </c>
       <c r="G16" s="2">
         <v>78279346</v>
+      </c>
+      <c r="H16" s="2">
+        <v>209124895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RV16: XGBoost v3 (chapisoletrain) 5000 trees
</commit_message>
<xml_diff>
--- a/Contabilidad modelos.xlsx
+++ b/Contabilidad modelos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\TODO\UNI ANDES\SEM 8 (2024-1)\Big Data y Machine Learning\Taller 3\BDML_2024_PS_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C47865-1E1C-483A-B234-BA27BC34EA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34848814-8669-4F74-8464-B98214A09784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4CAA7325-4791-4168-8C9B-C73AA3489A20}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t>No.</t>
   </si>
@@ -285,10 +285,13 @@
     <t>XGBoost</t>
   </si>
   <si>
-    <t>mtry: 40; tree depth: 4</t>
-  </si>
-  <si>
-    <t>mtry: 42; tree depth: 3</t>
+    <t>trees: 1000; mtry: 40; tree depth: 4</t>
+  </si>
+  <si>
+    <t>trees: 10000; mtry: 42; tree depth: 3</t>
+  </si>
+  <si>
+    <t>trees: 10000; mtry: 41; tree depth: 3</t>
   </si>
 </sst>
 </file>
@@ -699,11 +702,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B44E75D-B032-48F0-BA17-754A2F99A73B}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1113,6 +1116,32 @@
       </c>
       <c r="H16" s="2">
         <v>209124895</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="2">
+        <v>103713712</v>
+      </c>
+      <c r="H17" s="2">
+        <v>201455776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RV22: XGBoost LR: 0.00125
</commit_message>
<xml_diff>
--- a/Contabilidad modelos.xlsx
+++ b/Contabilidad modelos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/mc_arias1074_uniandes_edu_co/Documents/MSc Economics/Big Data &amp; Machine Learning/Problem set 3/carpeta equipo/BDML_2024_PS_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\TODO\UNI ANDES\SEM 8 (2024-1)\Big Data y Machine Learning\Taller 3\BDML_2024_PS_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{34848814-8669-4F74-8464-B98214A09784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F5E1BDA-7531-4FB4-8972-8E3659ED9D9D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB29A1C0-231C-440F-BBA5-D01FC951F2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="0" windowWidth="20460" windowHeight="10770" xr2:uid="{4CAA7325-4791-4168-8C9B-C73AA3489A20}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4CAA7325-4791-4168-8C9B-C73AA3489A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t>No.</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>trees: 8000; mtry: 28; tree depth: 4</t>
+  </si>
+  <si>
+    <t>Learning rate: 0.00125; trees: 2000; mtry: 28; tree depth: 5</t>
   </si>
 </sst>
 </file>
@@ -430,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,7 +450,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -763,24 +766,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B44E75D-B032-48F0-BA17-754A2F99A73B}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,7 +809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -832,7 +835,7 @@
         <v>212810609</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -858,7 +861,7 @@
         <v>204893397</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -881,7 +884,7 @@
         <v>159926333</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -904,7 +907,7 @@
         <v>165197347</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -927,7 +930,7 @@
         <v>155316466</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -947,7 +950,7 @@
         <v>156457892</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -974,7 +977,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>202325783</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>153274279</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>204342284</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>202804667</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>202034162</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>202821306</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>203713789</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>209124895</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1205,14 +1208,14 @@
         <v>201455776</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" t="s">
         <v>47</v>
       </c>
       <c r="D18" t="s">
@@ -1228,14 +1231,14 @@
         <v>72977310</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" t="s">
         <v>50</v>
       </c>
       <c r="D19" t="s">
@@ -1254,14 +1257,14 @@
         <v>205291202</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" t="s">
         <v>53</v>
       </c>
       <c r="D20" t="s">
@@ -1280,14 +1283,14 @@
         <v>202077458</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" t="s">
         <v>50</v>
       </c>
       <c r="D21" t="s">
@@ -1306,14 +1309,14 @@
         <v>202909139</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" t="s">
         <v>53</v>
       </c>
       <c r="D22" t="s">
@@ -1330,6 +1333,32 @@
       </c>
       <c r="H22" s="2">
         <v>202972185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="2">
+        <v>147278150</v>
+      </c>
+      <c r="H23" s="2">
+        <v>211139293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RV25: XGBoost + variables Intento de Red Neuronal
</commit_message>
<xml_diff>
--- a/Contabilidad modelos.xlsx
+++ b/Contabilidad modelos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/556f8df1e8c802cc/Documentos/BDML_2024/BDML_2024/BDML_2024_PS_3_definitivo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\TODO\UNI ANDES\SEM 8 (2024-1)\Big Data y Machine Learning\Taller 3\BDML_2024_PS_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{34848814-8669-4F74-8464-B98214A09784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FFCBFF2-FFB1-4171-9693-023BE15A5D49}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E615035D-C6B0-40F6-A2ED-148054016652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39405" yWindow="2340" windowWidth="22995" windowHeight="13245" xr2:uid="{4CAA7325-4791-4168-8C9B-C73AA3489A20}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4CAA7325-4791-4168-8C9B-C73AA3489A20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
   <si>
     <t>No.</t>
   </si>
@@ -353,14 +353,32 @@
   <si>
     <t>trees: 8000; mtry: 28; tree depth: 4</t>
   </si>
+  <si>
+    <t>update_role(property_type,  area, dist_nearest_restaurant,
+                dist_nearest_parques, baños, n_pisos_numerico,dist_nearest_universidades,
+                terraza, ascensor, estrato, dis_centro, dis_andino,
+                restaurant_1km, parques_1km, discotecas_1km, colegios_1km,
+                iluminado, exterior, remodelado, restaurant_300m, parques_300m,
+                discotecas_300m, colegios_300m, restaurant_100m, parques_100m, 
+                discotecas_100m, colegios_100m,</t>
+  </si>
+  <si>
+    <t>property_type,  area, dist_nearest_restaurant,
+                dist_nearest_parques, baños, n_pisos_numerico,dist_nearest_universidades,
+                terraza, ascensor, estrato, dis_centro, dis_andino,
+                restaurant_1km, parques_1km, discotecas_1km, colegios_1km,
+                iluminado, exterior, remodelado, restaurant_300m, parques_300m,
+                discotecas_300m, colegios_300m, restaurant_100m, parques_100m, 
+                discotecas_100m, colegios_100m,</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -419,17 +437,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,7 +465,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -762,14 +781,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B44E75D-B032-48F0-BA17-754A2F99A73B}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="111" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
@@ -1329,6 +1348,32 @@
       </c>
       <c r="H22" s="2">
         <v>202972185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="2">
+        <v>63366019</v>
+      </c>
+      <c r="H23" s="2">
+        <v>199574167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>